<commit_message>
miglioramenti ambiente test e altre modifiche generali
</commit_message>
<xml_diff>
--- a/test/test1.xlsx
+++ b/test/test1.xlsx
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2527263eb91b0b56/Desktop/TESI MAGISTRALE/ProveBenchmarking/ClusterVNS/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_2BB1D69C5B70DC736BB8261159F828704C93E343" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A49E3A32-ED36-4F94-8A2D-B9034DF6F323}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_2BB1D69C5B30534E277B2C11595770F248A5FD13" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D60E67DC-B87A-45A2-9C25-43460D28E306}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>file</t>
   </si>
@@ -84,6 +71,33 @@
   </si>
   <si>
     <t>feasible</t>
+  </si>
+  <si>
+    <t>time_execution</t>
+  </si>
+  <si>
+    <t>WorstValue</t>
+  </si>
+  <si>
+    <t>BestValue</t>
+  </si>
+  <si>
+    <t>averageValue</t>
+  </si>
+  <si>
+    <t>medianValue</t>
+  </si>
+  <si>
+    <t>WorstTime</t>
+  </si>
+  <si>
+    <t>bestTime</t>
+  </si>
+  <si>
+    <t>averageTime</t>
+  </si>
+  <si>
+    <t>medianTimes</t>
   </si>
   <si>
     <t>local_search_metaheuristic</t>
@@ -464,13 +478,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -525,7 +542,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -540,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
@@ -559,316 +576,201 @@
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>882.96682651529704</v>
+        <v>980.00663370079292</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
+      <c r="C9">
+        <v>3.3973781999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>873.55492671743946</v>
+        <v>994.07580503934173</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
+      <c r="C10">
+        <v>3.1545473000000008</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>865.31966109133498</v>
+        <v>927.42687223693713</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>873.8018119050671</v>
-      </c>
-      <c r="B12" t="b">
-        <v>1</v>
+      <c r="C11">
+        <v>3.2279993999999999</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>867.97690302493174</v>
-      </c>
-      <c r="B13" t="b">
-        <v>1</v>
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>862.4932225600204</v>
-      </c>
-      <c r="B14" t="b">
-        <v>1</v>
+        <v>994.07580503934173</v>
+      </c>
+      <c r="B14">
+        <v>927.42687223693713</v>
+      </c>
+      <c r="C14">
+        <v>967.16977032569059</v>
+      </c>
+      <c r="D14">
+        <v>980.00663370079292</v>
       </c>
       <c r="E14">
-        <f>AVERAGE(A9:A38)</f>
-        <v>889.79935189451862</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>878.52167424106619</v>
-      </c>
-      <c r="B15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>856.15464648110526</v>
-      </c>
-      <c r="B16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>865.31966109133498</v>
-      </c>
-      <c r="B17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>870.05286340640566</v>
-      </c>
-      <c r="B18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.3973781999999999</v>
+      </c>
+      <c r="F14">
+        <v>3.1545473000000008</v>
+      </c>
+      <c r="G14">
+        <v>3.2599749666666669</v>
+      </c>
+      <c r="H14">
+        <v>3.2279993999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>880.32381191267552</v>
-      </c>
-      <c r="B19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>893.47329347915365</v>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>915.32655841903511</v>
-      </c>
-      <c r="B21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>919.80452365283156</v>
+        <v>782</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>885.52777136168368</v>
-      </c>
-      <c r="B23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>891.71164273273575</v>
-      </c>
-      <c r="B24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>10.0131996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>886.93854831030342</v>
-      </c>
-      <c r="B25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>856.15464648110515</v>
-      </c>
-      <c r="B26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1003.130696738007</v>
-      </c>
-      <c r="B27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>867.17269303302589</v>
-      </c>
-      <c r="B28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>872.39187528406558</v>
-      </c>
-      <c r="B29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>873.80181190506698</v>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>964.37328448648213</v>
-      </c>
-      <c r="B31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>911.03317637528153</v>
-      </c>
-      <c r="B32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>870.35165333109364</v>
-      </c>
-      <c r="B33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>861.26258497682238</v>
-      </c>
-      <c r="B34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>869.24571943505384</v>
-      </c>
-      <c r="B35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>878.52167424106631</v>
-      </c>
-      <c r="B36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>898.65632603503582</v>
-      </c>
-      <c r="B37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>998.61606761103144</v>
-      </c>
-      <c r="B38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>15</v>
-      </c>
-      <c r="B42">
-        <v>6</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="b">
-        <v>0</v>
+        <v>782</v>
+      </c>
+      <c r="B25">
+        <v>782</v>
+      </c>
+      <c r="C25">
+        <v>782</v>
+      </c>
+      <c r="D25">
+        <v>782</v>
+      </c>
+      <c r="E25">
+        <v>10.0131996</v>
+      </c>
+      <c r="F25">
+        <v>10.0131996</v>
+      </c>
+      <c r="G25">
+        <v>10.0131996</v>
+      </c>
+      <c r="H25">
+        <v>10.0131996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>